<commit_message>
ogre2 not mapped error solved. New cam topic for each test added. New cam calibration added f18, f35, f70. Cameras also added
</commit_message>
<xml_diff>
--- a/Simulations/Tests/Angle_Img.xlsx
+++ b/Simulations/Tests/Angle_Img.xlsx
@@ -190,7 +190,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.9"/>
@@ -249,7 +249,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="33.2"/>

</xml_diff>